<commit_message>
Com a configuração do Utilizador feita
</commit_message>
<xml_diff>
--- a/Projeto_ES_87895_88047/Defeitos.xlsx
+++ b/Projeto_ES_87895_88047/Defeitos.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jreis\Dropbox\2019-2020 1Sem - Engenharia de Software I - SHARED\Projeto\Ficheiros projeto\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6112896D-8A6C-41CA-9C24-D83FEC65CC1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1EF5A43A-B425-4A37-909D-E259FF3D326E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="long-method" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'long-method'!$A$1:$M$421</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3402,48 +3398,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Cor1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Cor2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Cor3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Cor4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Cor5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Cor6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Cor1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Cor2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Cor3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Cor4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Cor5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Cor6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Cor1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Cor2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Cor3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Cor4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Cor5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Cor6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula Ligada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Cor1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Cor2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Cor3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Cor4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Cor5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Cor6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Correto" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Verificar Célula" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3459,7 +3455,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3758,8 +3754,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L421"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>